<commit_message>
The configuration table function is completed.
</commit_message>
<xml_diff>
--- a/Assets/ArtRes/Excel/游戏初始化配置表.xlsx
+++ b/Assets/ArtRes/Excel/游戏初始化配置表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="10480"/>
+    <workbookView windowWidth="13070" windowHeight="4410"/>
   </bookViews>
   <sheets>
     <sheet name="PlayerInfo" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
   <si>
     <t>主键</t>
   </si>
@@ -40,6 +40,9 @@
     <t>血量</t>
   </si>
   <si>
+    <t>攻击力</t>
+  </si>
+  <si>
     <t>治疗量</t>
   </si>
   <si>
@@ -58,6 +61,9 @@
     <t>health</t>
   </si>
   <si>
+    <t>attack</t>
+  </si>
+  <si>
     <t>curativeDose</t>
   </si>
   <si>
@@ -82,15 +88,9 @@
     <t>只因哥</t>
   </si>
   <si>
-    <t>伤害</t>
-  </si>
-  <si>
     <t>移速</t>
   </si>
   <si>
-    <t>attack</t>
-  </si>
-  <si>
     <t>speed</t>
   </si>
   <si>
@@ -100,7 +100,7 @@
     <t>Ghost</t>
   </si>
   <si>
-    <t>Monster</t>
+    <t>Phantom</t>
   </si>
   <si>
     <t>Shadow</t>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>发射速度</t>
+  </si>
+  <si>
+    <t>damage</t>
   </si>
   <si>
     <t>bulletNum</t>
@@ -1068,20 +1071,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="6"/>
   <cols>
     <col min="4" max="4" width="13.4545454545455" customWidth="1"/>
-    <col min="5" max="5" width="12.3636363636364" customWidth="1"/>
+    <col min="5" max="5" width="14.0909090909091" customWidth="1"/>
     <col min="6" max="6" width="13.3636363636364" customWidth="1"/>
+    <col min="7" max="7" width="13.7272727272727" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1100,69 +1104,81 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C5">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
         <v>1</v>
       </c>
-      <c r="E5">
-        <v>10</v>
-      </c>
       <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
         <v>0.3</v>
       </c>
     </row>
@@ -1178,8 +1194,8 @@
   <sheetPr/>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="7" outlineLevelCol="4"/>
@@ -1195,24 +1211,24 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
         <v>20</v>
@@ -1220,24 +1236,24 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1321,7 +1337,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="5" outlineLevelCol="5"/>
@@ -1354,47 +1370,47 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1402,7 +1418,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5">
         <v>0.4</v>
@@ -1422,7 +1438,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C6">
         <v>0.15</v>

</xml_diff>